<commit_message>
completed extent report with screenshot
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/view_cart/datasheet/login.xlsx
+++ b/src/main/java/com/qa/view_cart/datasheet/login.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14030" windowHeight="2190" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
   <si>
     <t>Expected Result</t>
   </si>
@@ -542,10 +543,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -578,6 +579,14 @@
         <v>17</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>